<commit_message>
Updates to fairagro templates
</commit_message>
<xml_diff>
--- a/templates/community/FAIRagro/Agronomy_-_Fields/Agronomy_-_Fields_v1.0.0.xlsx
+++ b/templates/community/FAIRagro/Agronomy_-_Fields/Agronomy_-_Fields_v1.0.0.xlsx
@@ -1,30 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2833CDAD-B734-47F7-AC44-ECDC834C6A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="isa_template" sheetId="1" r:id="rId1"/>
-    <sheet name="Materials-Fields" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" name="isa_template" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Materials-Fields" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -67,6 +50,9 @@
     <t>Table</t>
   </si>
   <si>
+    <t>Materials-Fields</t>
+  </si>
+  <si>
     <t>ERS</t>
   </si>
   <si>
@@ -382,7 +368,7 @@
     <t>Term Accession Number (AGRO:00000623)</t>
   </si>
   <si>
-    <t>Output [Source Name]</t>
+    <t>Output [Sample Name]</t>
   </si>
   <si>
     <t/>
@@ -482,22 +468,19 @@
   </si>
   <si>
     <t>220</t>
-  </si>
-  <si>
-    <t>Materials-Fields</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -540,8 +523,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="annotationTable" displayName="annotationTable" ref="A1:BN2">
-  <autoFilter ref="A1:BN2" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:BN2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:BN2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -610,72 +593,72 @@
     <filterColumn colId="65" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="66">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Input [Source Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Characteristic [Locality]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Term Source REF (bco:locality)"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Term Accession Number (bco:locality)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Characteristic [Country]"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Term Source REF (bco:country)"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Term Accession Number (bco:country)"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Characteristic [State Province]"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Term Source REF (bco:stateProvince)"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Term Accession Number (bco:stateProvince)"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Characteristic [County]"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Term Source REF (bco:county)"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Term Accession Number (bco:county)"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Parameter [Decimal Latitude]"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Term Source REF (bco:decimalLatitude)"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Term Accession Number (bco:decimalLatitude)"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Parameter [Decimal Longitude]"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Term Source REF (bco:decimalLongitude)"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Term Accession Number (bco:decimalLongitude)"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Parameter [Maximum Elevation In Meters]"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Unit"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Term Source REF (bco:maximumElevationInMeters)"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Term Accession Number (bco:maximumElevationInMeters)"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Parameter [slope]"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Unit "/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Term Source REF ()"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Term Accession Number ()"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Characteristic [slope orientation]"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Term Source REF (AGRO:00000328)"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Term Accession Number (AGRO:00000328)"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Parameter [slope length]"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Unit  "/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Term Source REF () "/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Term Accession Number () "/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Parameter [field rockiness]"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Unit   "/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Term Source REF (AGRO:00000666)"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Term Accession Number (AGRO:00000666)"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Parameter [field area]"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Unit    "/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Term Source REF (AGRO:00000300)"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Term Accession Number (AGRO:00000300)"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Parameter [field obstruction to sun]"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Unit     "/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Term Source REF ()  "/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Term Accession Number ()  "/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Characteristic [drainage process]"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Term Source REF (ENVO:01003009)"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Term Accession Number (ENVO:01003009)"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Parameter [drainage depth]"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Unit      "/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Term Source REF ()   "/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Term Accession Number ()   "/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="Parameter [drain spacing]"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="Unit       "/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="Term Source REF ()    "/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="Term Accession Number ()    "/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="Parameter [drain radius]"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="Unit        "/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="Term Source REF ()     "/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="Term Accession Number ()     "/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="Parameter [distance between a weather station and the field]"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="Unit         "/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="Term Source REF (AGRO:00000623)"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="Term Accession Number (AGRO:00000623)"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="Output [Source Name]"/>
+    <tableColumn id="1" name="Input [Source Name]" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Characteristic [Locality]" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Term Source REF (bco:locality)" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Term Accession Number (bco:locality)" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Characteristic [Country]" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Term Source REF (bco:country)" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Term Accession Number (bco:country)" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Characteristic [State Province]" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Term Source REF (bco:stateProvince)" totalsRowFunction="none"/>
+    <tableColumn id="10" name="Term Accession Number (bco:stateProvince)" totalsRowFunction="none"/>
+    <tableColumn id="11" name="Characteristic [County]" totalsRowFunction="none"/>
+    <tableColumn id="12" name="Term Source REF (bco:county)" totalsRowFunction="none"/>
+    <tableColumn id="13" name="Term Accession Number (bco:county)" totalsRowFunction="none"/>
+    <tableColumn id="14" name="Parameter [Decimal Latitude]" totalsRowFunction="none"/>
+    <tableColumn id="15" name="Term Source REF (bco:decimalLatitude)" totalsRowFunction="none"/>
+    <tableColumn id="16" name="Term Accession Number (bco:decimalLatitude)" totalsRowFunction="none"/>
+    <tableColumn id="17" name="Parameter [Decimal Longitude]" totalsRowFunction="none"/>
+    <tableColumn id="18" name="Term Source REF (bco:decimalLongitude)" totalsRowFunction="none"/>
+    <tableColumn id="19" name="Term Accession Number (bco:decimalLongitude)" totalsRowFunction="none"/>
+    <tableColumn id="20" name="Parameter [Maximum Elevation In Meters]" totalsRowFunction="none"/>
+    <tableColumn id="21" name="Unit" totalsRowFunction="none"/>
+    <tableColumn id="22" name="Term Source REF (bco:maximumElevationInMeters)" totalsRowFunction="none"/>
+    <tableColumn id="23" name="Term Accession Number (bco:maximumElevationInMeters)" totalsRowFunction="none"/>
+    <tableColumn id="24" name="Parameter [slope]" totalsRowFunction="none"/>
+    <tableColumn id="25" name="Unit " totalsRowFunction="none"/>
+    <tableColumn id="26" name="Term Source REF ()" totalsRowFunction="none"/>
+    <tableColumn id="27" name="Term Accession Number ()" totalsRowFunction="none"/>
+    <tableColumn id="28" name="Characteristic [slope orientation]" totalsRowFunction="none"/>
+    <tableColumn id="29" name="Term Source REF (AGRO:00000328)" totalsRowFunction="none"/>
+    <tableColumn id="30" name="Term Accession Number (AGRO:00000328)" totalsRowFunction="none"/>
+    <tableColumn id="31" name="Parameter [slope length]" totalsRowFunction="none"/>
+    <tableColumn id="32" name="Unit  " totalsRowFunction="none"/>
+    <tableColumn id="33" name="Term Source REF () " totalsRowFunction="none"/>
+    <tableColumn id="34" name="Term Accession Number () " totalsRowFunction="none"/>
+    <tableColumn id="35" name="Parameter [field rockiness]" totalsRowFunction="none"/>
+    <tableColumn id="36" name="Unit   " totalsRowFunction="none"/>
+    <tableColumn id="37" name="Term Source REF (AGRO:00000666)" totalsRowFunction="none"/>
+    <tableColumn id="38" name="Term Accession Number (AGRO:00000666)" totalsRowFunction="none"/>
+    <tableColumn id="39" name="Parameter [field area]" totalsRowFunction="none"/>
+    <tableColumn id="40" name="Unit    " totalsRowFunction="none"/>
+    <tableColumn id="41" name="Term Source REF (AGRO:00000300)" totalsRowFunction="none"/>
+    <tableColumn id="42" name="Term Accession Number (AGRO:00000300)" totalsRowFunction="none"/>
+    <tableColumn id="43" name="Parameter [field obstruction to sun]" totalsRowFunction="none"/>
+    <tableColumn id="44" name="Unit     " totalsRowFunction="none"/>
+    <tableColumn id="45" name="Term Source REF ()  " totalsRowFunction="none"/>
+    <tableColumn id="46" name="Term Accession Number ()  " totalsRowFunction="none"/>
+    <tableColumn id="47" name="Characteristic [drainage process]" totalsRowFunction="none"/>
+    <tableColumn id="48" name="Term Source REF (ENVO:01003009)" totalsRowFunction="none"/>
+    <tableColumn id="49" name="Term Accession Number (ENVO:01003009)" totalsRowFunction="none"/>
+    <tableColumn id="50" name="Parameter [drainage depth]" totalsRowFunction="none"/>
+    <tableColumn id="51" name="Unit      " totalsRowFunction="none"/>
+    <tableColumn id="52" name="Term Source REF ()   " totalsRowFunction="none"/>
+    <tableColumn id="53" name="Term Accession Number ()   " totalsRowFunction="none"/>
+    <tableColumn id="54" name="Parameter [drain spacing]" totalsRowFunction="none"/>
+    <tableColumn id="55" name="Unit       " totalsRowFunction="none"/>
+    <tableColumn id="56" name="Term Source REF ()    " totalsRowFunction="none"/>
+    <tableColumn id="57" name="Term Accession Number ()    " totalsRowFunction="none"/>
+    <tableColumn id="58" name="Parameter [drain radius]" totalsRowFunction="none"/>
+    <tableColumn id="59" name="Unit        " totalsRowFunction="none"/>
+    <tableColumn id="60" name="Term Source REF ()     " totalsRowFunction="none"/>
+    <tableColumn id="61" name="Term Accession Number ()     " totalsRowFunction="none"/>
+    <tableColumn id="62" name="Parameter [distance between a weather station and the field]" totalsRowFunction="none"/>
+    <tableColumn id="63" name="Unit         " totalsRowFunction="none"/>
+    <tableColumn id="64" name="Term Source REF (AGRO:00000623)" totalsRowFunction="none"/>
+    <tableColumn id="65" name="Term Accession Number (AGRO:00000623)" totalsRowFunction="none"/>
+    <tableColumn id="66" name="Output [Sample Name]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -977,19 +960,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -997,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1005,7 +985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1021,7 +1001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1029,603 +1009,600 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="V1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="W1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="X1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Y1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AB1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AC1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AD1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AE1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AF1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AG1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AH1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AI1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AJ1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AK1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AL1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AM1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AN1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AO1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AP1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AQ1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AR1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AS1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AT1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AU1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AV1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AW1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AX1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AY1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AZ1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="BA1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="BB1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="BC1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BD1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BE1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="BF1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BG1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="BH1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BI1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="BJ1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="BK1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="BL1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="BM1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="BN1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
         <v>119</v>
       </c>
-      <c r="C2" t="s">
-        <v>118</v>
-      </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" t="s">
+        <v>127</v>
+      </c>
+      <c r="O2" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>128</v>
+      </c>
+      <c r="R2" t="s">
+        <v>119</v>
+      </c>
+      <c r="S2" t="s">
+        <v>119</v>
+      </c>
+      <c r="T2" t="s">
+        <v>129</v>
+      </c>
+      <c r="U2" t="s">
+        <v>130</v>
+      </c>
+      <c r="V2" t="s">
+        <v>131</v>
+      </c>
+      <c r="W2" t="s">
+        <v>132</v>
+      </c>
+      <c r="X2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC2" t="s">
         <v>122</v>
       </c>
-      <c r="H2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K2" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" t="s">
-        <v>118</v>
-      </c>
-      <c r="M2" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" t="s">
-        <v>126</v>
-      </c>
-      <c r="O2" t="s">
-        <v>118</v>
-      </c>
-      <c r="P2" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>127</v>
-      </c>
-      <c r="R2" t="s">
-        <v>118</v>
-      </c>
-      <c r="S2" t="s">
-        <v>118</v>
-      </c>
-      <c r="T2" t="s">
-        <v>128</v>
-      </c>
-      <c r="U2" t="s">
-        <v>129</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="AD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF2" t="s">
         <v>130</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AG2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>131</v>
       </c>
-      <c r="X2" t="s">
+      <c r="BA2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BE2" t="s">
         <v>132</v>
       </c>
-      <c r="Y2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="BF2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>148</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>151</v>
+      </c>
+      <c r="BK2" t="s">
         <v>130</v>
       </c>
-      <c r="AA2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>136</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AH2" t="s">
+      <c r="BL2" t="s">
         <v>131</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="BM2" t="s">
         <v>132</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>148</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>149</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>131</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>149</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>147</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>148</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>150</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>130</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>131</v>
-      </c>
       <c r="BN2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>